<commit_message>
Changed upper limit of days of planning
</commit_message>
<xml_diff>
--- a/planning/benchmarks.xlsx
+++ b/planning/benchmarks.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Universiteit\Semester 8\APLAI\Git Project\APLAI\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unief\APLAI\Git Project\APLAI\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682A02B2-3AFA-45B1-AA3F-D04934D00477}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CB6CA2-8B56-4FBE-A00C-06D7AA9F5B4F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA6F14F0-FC13-4784-B34F-003BA60A0E94}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -70,8 +69,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,8 +106,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -415,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85DC67BB-8A15-45A3-BA37-C8860F8B1C4B}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +571,52 @@
         <v>478734</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f>AVERAGE(A2:A4)</f>
+        <v>578</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" ref="B5:K5" si="0">AVERAGE(B2:B4)</f>
+        <v>234.33333333333334</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>2396</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>79755</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>55297</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>1109.3333333333333</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>2760.3333333333335</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>6005.333333333333</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>8755.3333333333339</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>232396</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>475145.66666666669</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed some comments, and added planning benchmarks
</commit_message>
<xml_diff>
--- a/planning/benchmarks.xlsx
+++ b/planning/benchmarks.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Universiteit\Semester 8\APLAI\Git Project\APLAI\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unief\APLAI\Git Project\APLAI\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431EAB0E-DE15-49EA-80F8-518AA5993C07}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538A56EF-B218-4F93-819E-47608414E09E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16995" yWindow="690" windowWidth="10845" windowHeight="10605" xr2:uid="{DA6F14F0-FC13-4784-B34F-003BA60A0E94}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -432,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85DC67BB-8A15-45A3-BA37-C8860F8B1C4B}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,320 +480,326 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>390</v>
+        <v>250</v>
       </c>
       <c r="B2">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="C2">
-        <v>1531</v>
+        <v>938</v>
       </c>
       <c r="D2">
-        <v>37016</v>
+        <v>24031</v>
       </c>
       <c r="E2">
-        <v>24437</v>
+        <v>15625</v>
       </c>
       <c r="F2">
-        <v>328</v>
+        <v>219</v>
       </c>
       <c r="G2">
-        <v>328</v>
+        <v>219</v>
       </c>
       <c r="H2">
-        <v>516</v>
+        <v>313</v>
       </c>
       <c r="I2">
-        <v>6625</v>
+        <v>4171</v>
       </c>
       <c r="J2">
-        <v>6360</v>
+        <v>4016</v>
       </c>
       <c r="K2">
-        <v>75500</v>
+        <v>48469</v>
       </c>
       <c r="L2">
-        <v>5528609</v>
+        <v>3559000</v>
       </c>
       <c r="M2">
-        <v>6438</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>391</v>
+        <v>266</v>
       </c>
       <c r="B3">
-        <v>141</v>
+        <v>79</v>
       </c>
       <c r="C3">
-        <v>1812</v>
+        <v>937</v>
       </c>
       <c r="D3">
         <v>36171</v>
       </c>
       <c r="E3">
-        <v>24734</v>
+        <v>15672</v>
       </c>
       <c r="F3">
-        <v>344</v>
+        <v>203</v>
       </c>
       <c r="G3">
-        <v>313</v>
+        <v>218</v>
       </c>
       <c r="H3">
-        <v>484</v>
+        <v>328</v>
       </c>
       <c r="I3">
-        <v>6593</v>
+        <v>4204</v>
       </c>
       <c r="J3">
-        <v>6328</v>
+        <v>4047</v>
       </c>
       <c r="K3">
-        <v>77172</v>
+        <v>48437</v>
       </c>
       <c r="M3">
-        <v>6453</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>390</v>
+        <v>266</v>
       </c>
       <c r="B4">
-        <v>157</v>
+        <v>78</v>
       </c>
       <c r="C4">
-        <v>1516</v>
+        <v>938</v>
       </c>
       <c r="D4">
-        <v>40579</v>
+        <v>24078</v>
       </c>
       <c r="E4">
-        <v>25094</v>
+        <v>15656</v>
       </c>
       <c r="F4">
-        <v>328</v>
+        <v>219</v>
       </c>
       <c r="G4">
-        <v>328</v>
+        <v>219</v>
       </c>
       <c r="H4">
-        <v>516</v>
+        <v>344</v>
       </c>
       <c r="I4">
-        <v>6594</v>
+        <v>4171</v>
       </c>
       <c r="J4">
-        <v>6203</v>
+        <v>4062</v>
       </c>
       <c r="K4">
-        <v>75875</v>
+        <v>48438</v>
       </c>
       <c r="M4">
-        <v>6453</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>AVERAGE(A2:A4)</f>
-        <v>390.33333333333331</v>
+        <v>260.66666666666669</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" ref="B5:M5" si="0">AVERAGE(B2:B4)</f>
-        <v>146.33333333333334</v>
+        <v>83.333333333333329</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>1619.6666666666667</v>
+        <v>937.66666666666663</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>37922</v>
+        <v>28093.333333333332</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>24755</v>
+        <v>15651</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>333.33333333333331</v>
+        <v>213.66666666666666</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>323</v>
+        <v>218.66666666666666</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>505.33333333333331</v>
+        <v>328.33333333333331</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>6604</v>
+        <v>4182</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
-        <v>6297</v>
+        <v>4041.6666666666665</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>76182.333333333328</v>
+        <v>48448</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>5528609</v>
+        <v>3559000</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="0"/>
-        <v>6448</v>
+        <v>2114.6666666666665</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>625</v>
+        <v>438</v>
       </c>
       <c r="B7">
-        <v>375</v>
+        <v>281</v>
       </c>
       <c r="C7">
-        <v>2234</v>
+        <v>1578</v>
       </c>
       <c r="D7">
-        <v>85593</v>
+        <v>61063</v>
       </c>
       <c r="E7">
-        <v>3161516</v>
+        <v>2053172</v>
       </c>
       <c r="F7">
-        <v>7047</v>
+        <v>4687</v>
       </c>
       <c r="G7">
-        <v>329</v>
+        <v>219</v>
       </c>
       <c r="H7">
-        <v>484</v>
+        <v>313</v>
       </c>
       <c r="I7">
-        <v>8172</v>
+        <v>5407</v>
       </c>
       <c r="J7">
-        <v>15625</v>
+        <v>10437</v>
+      </c>
+      <c r="K7">
+        <v>222703</v>
+      </c>
+      <c r="L7">
+        <v>7793156</v>
       </c>
       <c r="M7">
-        <v>7157609</v>
+        <v>4693625</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>657</v>
+        <v>469</v>
       </c>
       <c r="B8">
-        <v>407</v>
+        <v>281</v>
       </c>
       <c r="C8">
-        <v>2312</v>
+        <v>1531</v>
       </c>
       <c r="D8">
-        <v>86407</v>
+        <v>60906</v>
       </c>
       <c r="F8">
-        <v>7172</v>
+        <v>4688</v>
       </c>
       <c r="G8">
-        <v>328</v>
+        <v>219</v>
       </c>
       <c r="H8">
-        <v>500</v>
+        <v>313</v>
       </c>
       <c r="I8">
-        <v>8063</v>
+        <v>5375</v>
       </c>
       <c r="J8">
-        <v>16938</v>
+        <v>10453</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>671</v>
+        <v>453</v>
       </c>
       <c r="B9">
-        <v>390</v>
+        <v>281</v>
       </c>
       <c r="C9">
-        <v>2329</v>
+        <v>1547</v>
       </c>
       <c r="D9">
-        <v>85953</v>
+        <v>62594</v>
       </c>
       <c r="F9">
-        <v>6890</v>
+        <v>4687</v>
       </c>
       <c r="G9">
-        <v>328</v>
+        <v>234</v>
       </c>
       <c r="H9">
-        <v>469</v>
+        <v>343</v>
       </c>
       <c r="I9">
-        <v>8156</v>
+        <v>5375</v>
       </c>
       <c r="J9">
-        <v>15578</v>
+        <v>10422</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>AVERAGE(A7:A9)</f>
-        <v>651</v>
+        <v>453.33333333333331</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" ref="B10:C10" si="1">AVERAGE(B7:B9)</f>
-        <v>390.66666666666669</v>
+        <v>281</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>2291.6666666666665</v>
+        <v>1552</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" ref="D10" si="2">AVERAGE(D7:D9)</f>
-        <v>85984.333333333328</v>
+        <v>61521</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ref="E10" si="3">AVERAGE(E7:E9)</f>
-        <v>3161516</v>
+        <v>2053172</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" ref="F10" si="4">AVERAGE(F7:F9)</f>
-        <v>7036.333333333333</v>
+        <v>4687.333333333333</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" ref="G10" si="5">AVERAGE(G7:G9)</f>
-        <v>328.33333333333331</v>
+        <v>224</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" ref="H10" si="6">AVERAGE(H7:H9)</f>
-        <v>484.33333333333331</v>
+        <v>323</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" ref="I10" si="7">AVERAGE(I7:I9)</f>
-        <v>8130.333333333333</v>
+        <v>5385.666666666667</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" ref="J10" si="8">AVERAGE(J7:J9)</f>
-        <v>16047</v>
-      </c>
-      <c r="K10" s="1" t="e">
+        <v>10437.333333333334</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" ref="K10" si="9">AVERAGE(K7:K9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="1" t="e">
+        <v>222703</v>
+      </c>
+      <c r="L10" s="1">
         <f t="shared" ref="L10" si="10">AVERAGE(L7:L9)</f>
-        <v>#DIV/0!</v>
+        <v>7793156</v>
       </c>
       <c r="M10" s="1">
         <f t="shared" ref="M10" si="11">AVERAGE(M7:M9)</f>
-        <v>7157609</v>
+        <v>4693625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>